<commit_message>
New data for A2-A6, + B5-B7
</commit_message>
<xml_diff>
--- a/IvVasil/evidence.xlsx
+++ b/IvVasil/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176" firstSheet="1" activeTab="23"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -33,13 +33,14 @@
     <sheet name="B2" sheetId="24" r:id="rId24"/>
     <sheet name="B5" sheetId="25" r:id="rId25"/>
     <sheet name="B6" sheetId="26" r:id="rId26"/>
+    <sheet name="B7" sheetId="27" r:id="rId27"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="126">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -104,18 +105,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>A4</t>
   </si>
   <si>
     <t>A5</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
     <t>A6</t>
   </si>
   <si>
@@ -140,15 +135,6 @@
     <t>A13</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>A14</t>
   </si>
   <si>
@@ -173,12 +159,6 @@
     <t>B1</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>B2</t>
   </si>
   <si>
@@ -215,42 +195,18 @@
     <t>stakingrewards</t>
   </si>
   <si>
-    <t>nft1</t>
-  </si>
-  <si>
-    <t>D958D283C49CD0C65A65958EFE9FBD9BD5ABA0CECDCE69406D993B3BF0EC1E95</t>
-  </si>
-  <si>
-    <t>B1E7DA3A9DB9B8D9C17120237AE37A1009DF95CA419C4E313DB0292997BCCE21</t>
-  </si>
-  <si>
-    <t>nft2</t>
-  </si>
-  <si>
-    <t>9F50CCE36798B91B8802282A3DF0A297043DCEC9919417D7F586395D8EC2F88B</t>
-  </si>
-  <si>
     <t>elgafar-1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>stars1lnnccnwm2rkk9nngr3pfekf63q5m2qmw4txftu4pyv9tr0cpzxrqfydqh3</t>
   </si>
   <si>
-    <t>1EDD62029BC10D4C851C7C7F7E3754194471A0BD5CC885C6E8B0B36B960B6F5E</t>
-  </si>
-  <si>
     <t>ibc/454B7203F4932E12B135D5E43870DA0C648EA8890E5AB734CA4EA5C7D9B2FF01</t>
   </si>
   <si>
     <t>uptick_7000-2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>D5D919A240067D14A1B10360A1D5F0365528478591E1EFBD704B20CF45CFDBC6</t>
-  </si>
-  <si>
-    <t>241DF64297B447719DC9D559B5895F1E14A1BA82225D91E85263F61F7701B30F</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>3DB7F2B3A9DEE33D93DE155057F8B0FF055D2F9167EE4666E611EDF7BB00EB7F</t>
@@ -263,17 +219,226 @@
   </si>
   <si>
     <t>DE46FAEE6BD154686E59B61A9B9C6DCFB04AF866C0F63D09BC450527E5A41A44</t>
+  </si>
+  <si>
+    <t>56A282E67B40D0A5D446CE07E9E9BC3BE3BE09E69279AF67006EFA2DB57E2685</t>
+  </si>
+  <si>
+    <t>8B16DFC3D6AE6F5D12526D13F1937822F4997D7722AD08BB840C42B2F974B883</t>
+  </si>
+  <si>
+    <t>ibc/ACC4F9914FCC8D170A6A229D792EBCA7B9CAA61316B0A950AB36841839E82855</t>
+  </si>
+  <si>
+    <t>nftstage27</t>
+  </si>
+  <si>
+    <t>nftstage28</t>
+  </si>
+  <si>
+    <t>nftstage29</t>
+  </si>
+  <si>
+    <t>nftstage210</t>
+  </si>
+  <si>
+    <t>nftstage211</t>
+  </si>
+  <si>
+    <t>nftstage212</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>8F4DD7078AAA7974314746093DBC173AE7B09D56358F2D8AD90ECB8036191CA5</t>
+  </si>
+  <si>
+    <t>ECCB1FCAEDED05AC8CB5C60CE8C626B76E0B8AB783A96246A816AF83F9617DFB</t>
+  </si>
+  <si>
+    <t>269B04B92D95DCA266F11B9BE8BE6D2A9B2B7CAB18534E7DA28EB25069734455</t>
+  </si>
+  <si>
+    <t>1B7CF4C05AF15600E7F8E7B775B867B0C8FC8425A4B68AF21E4FBE34BF0ED3D5</t>
+  </si>
+  <si>
+    <t>3534C99CA1C071A9D0F9191A7102498425E93676F23ED7E8F976B6B18A2FCC89</t>
+  </si>
+  <si>
+    <t>0A8FB8E9021A4E8FD132AC2B734F03EA01B83A0A20B3279857CDD2158C757C27</t>
+  </si>
+  <si>
+    <t>ibc/B16AC752B3FD36313F0385FF568FB6F117097DE29B8D8A6A6710BCD499A2C668</t>
+  </si>
+  <si>
+    <t>ibc/7B5849E281C0242D4336372F5D5F0E8A8CCC994BED1BCC541518E405122765C0</t>
+  </si>
+  <si>
+    <t>ibc/CCCE0094A6A63C21138C830925F0F90B1A62861675F79F91FBB8B90F0C863E2E</t>
+  </si>
+  <si>
+    <t>ibc/AA99DECC76DAC0C3C79F60D07FB73D7F8E6B99C7BB8236B124A18A30C0D558F4</t>
+  </si>
+  <si>
+    <t>ibc/27F1ABABB080D1D9AC994F9909CEDB56FC362CAC77113D39EBB48240AE2F2D40</t>
+  </si>
+  <si>
+    <t>D03D15B837FBA4661CD9AD5C4E544AD605EE6E018DE701DC0A41913069E62E2C</t>
+  </si>
+  <si>
+    <t>62B5B7735D37373180B95A7912B21D547CDC7FC2F939CB9D07940C69ABDA8C2B</t>
+  </si>
+  <si>
+    <t>F28D05A082A33CC935AFD1F18C4ED55FAF4207AC4F79B14541DF73CACFEB71E6</t>
+  </si>
+  <si>
+    <t>06E15167F8F664801A28ED4BA09C05E402205317F3BA90E0443582AF042BB212</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>9426DF54C99A38B5DF5F2CFE1524F5AFD516E41F616870DE572B56E84E21D730</t>
+  </si>
+  <si>
+    <t>65C79E30E94075E96696A27DF49F4806B5899B5FD2F18E679415D635A62CD8B1</t>
+  </si>
+  <si>
+    <t>1E6050A83E05437C93A5E33FE71C64327F56018178E4E22FD729676D3648AA6A</t>
+  </si>
+  <si>
+    <t>637A24ED9F39633280BA383EA34F223BEB1DFF9A326C9F97C64E22E42706685F</t>
+  </si>
+  <si>
+    <t>212BC0316D34BF58AB69D8CED409D0CF14D93503D319D190222C12B54FF82EF7</t>
+  </si>
+  <si>
+    <t>AA355BA4B5135C9C09D089E23FFDAAC00C753F51AB3ABDA5DEC2C20659FE7442</t>
+  </si>
+  <si>
+    <t>F15340E1D84647BED0F9A3B74A4C76C0FA3974B46A2BF5C4D96A4DEAE5BB091E</t>
+  </si>
+  <si>
+    <t>1DDF327C4220D0A62A0C182B4AC17EA2BCD46D95801643286A7E4F1C99CD8DE0</t>
+  </si>
+  <si>
+    <t>22A9522F0D357C274AA5D7A06D72A5C33232DD4DEE9F9286900E86486372845C</t>
+  </si>
+  <si>
+    <t>5A6BDAFE4CAD673D288C687A96F0622E4CA3A02DC69DE37E82E07C7348C5E445</t>
+  </si>
+  <si>
+    <t>ADF6DCAC49BF2F60EB006E56728A6298414B2C99DD000CB30F12C5F0DAB60DE0</t>
+  </si>
+  <si>
+    <t>572894AC46CBB97ABCCD527E4539091896D715CA5DD911FA35D140F59A47D838</t>
+  </si>
+  <si>
+    <t>E69C6CB58ED9C133AC4E616A2F94B78E12B2FB850D4B085DA6922BB2473D8673</t>
+  </si>
+  <si>
+    <t>1A4AC7DF0EA716EDEC091572ABADC3EA498D2403F9D147DFF9A5B606096DF1B4</t>
+  </si>
+  <si>
+    <t>5A04CE9603E6658539E0DCE1FBA3BF198519EF9D445FB8853A36AC6FFFB20319</t>
+  </si>
+  <si>
+    <t>DEA13D7D980AB3DD85D4B7DE0ED4D1A7B308268C9794B62D52A62D8C85637394</t>
+  </si>
+  <si>
+    <t>051F3ABD62697104CC1BA6B110DCDE52037E13F439201ECC69307D47235B4A99</t>
+  </si>
+  <si>
+    <t>83CD4136A6CCBF9DA5EE9DF42E30D4F173C3CE5804C2B90DEE0AFD0CF02756AA</t>
+  </si>
+  <si>
+    <t>B4A54C61E0F8BA810F5104A270C5505DC77446F251A7DF350B0178E70DA18E29</t>
+  </si>
+  <si>
+    <t>DF099EB52E431D1841D85D8AE06804D7B44F25440D1C84663D7522FD06A096D0</t>
+  </si>
+  <si>
+    <t>5FC8DB976A038479F5AA79203892AF911860B33C3119A67B9B3B4063FE24AF3D</t>
+  </si>
+  <si>
+    <t>EC21CB6D8B502A4DB42969BBF5C4EA0DDA3CB98F4E4431AEBCF94AD484E2D49A</t>
+  </si>
+  <si>
+    <t>C7EEBD8F7F86C17BFF4656AF78E651375AF86F1642341507403069F236D503A5</t>
+  </si>
+  <si>
+    <t>F65920384AF32E48290FA1C6CCDE2C0991150E6915913C1877A6763CD2900A95</t>
+  </si>
+  <si>
+    <t>B8F4AB15C602FB4C0FD96B07531E3EC71848520D3B77A85D48F5CA458D0B05C7</t>
+  </si>
+  <si>
+    <t>1EACB2F9F287890B1F0557B7C19BC81916E375CA93419A4901FFE194E9A44C87</t>
+  </si>
+  <si>
+    <t>99B89C36A78252B4F284295D42A9022C589AC72679EBB556189AC6C5BA970E23</t>
+  </si>
+  <si>
+    <t>0408A282B85C082A47EE6424BB3A5C19C53E946F523DA7C7DD56864E0B94524E</t>
+  </si>
+  <si>
+    <t>98072C9F3D97972A4842F551A1163ADB6183B81F0E40005AEEC580E58DDBDB14</t>
+  </si>
+  <si>
+    <t>9CD13209E7F8BE3D7EA952BEC74A87227C3DCE732F6F308FA9EC3B0A50D0D403</t>
+  </si>
+  <si>
+    <t>301F40F0D84DF604B3129F915562CF9CF46BA4224BE3E670EB49D46272A836CF</t>
+  </si>
+  <si>
+    <t>42295C33E2D28FC50C99B8C036E363DFC737E22696E38BE03EF8785554E357F6</t>
+  </si>
+  <si>
+    <t>nftA2</t>
+  </si>
+  <si>
+    <t>nftA1</t>
+  </si>
+  <si>
+    <t>53E3293D158D98D52FE5688E468925B7D86883ECC9C7D79AC7A0BE3731F45193</t>
+  </si>
+  <si>
+    <t>D69AFDF46CC8E9C873942087EE821955F4F08081CB9C126A867D4C38FEDD68FC</t>
+  </si>
+  <si>
+    <t>5BFE48A9507361A2D85F68FD7B243DB729798610DC414E8A061D3BDC0E6A39B6</t>
+  </si>
+  <si>
+    <t>46C9AE135CE85FE9562CC3B082911465651AAC4C5B66D94ACB281019E20FEB64</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -314,6 +479,27 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -427,30 +613,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -462,7 +651,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -474,19 +663,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="3"/>
+    <cellStyle name="Обычный 3" xfId="4"/>
+    <cellStyle name="Обычный 4" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1645,20 +1849,20 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="4" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
+    <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1">
+      <c r="B3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-    </row>
-    <row r="7" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+    </row>
+    <row r="7" spans="2:4" ht="17.399999999999999">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1669,14 +1873,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="15">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="15">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -1685,14 +1889,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="15">
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="15">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>5</v>
@@ -1701,14 +1905,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="15">
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" ht="15">
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
         <v>5</v>
@@ -1717,14 +1921,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="15">
       <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="15">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -1733,340 +1937,340 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="15">
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="15">
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="15">
+      <c r="B19" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="15">
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="15">
+      <c r="B21" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="15">
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="15">
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="15">
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="15">
       <c r="B25" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="15">
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="15">
       <c r="B27" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" ht="15">
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="15">
       <c r="B29" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="15">
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="15">
       <c r="B31" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" ht="15">
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="15">
       <c r="B33" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" ht="15">
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="15">
       <c r="B35" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" ht="15">
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="15">
       <c r="B37" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" ht="15">
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="15">
       <c r="B39" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" ht="15">
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="15">
       <c r="B41" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" ht="15">
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="15">
       <c r="B43" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" ht="15">
       <c r="B44" s="3"/>
       <c r="C44" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="15">
       <c r="B45" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" ht="15">
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="15">
       <c r="B47" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" ht="15">
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" ht="15">
       <c r="B49" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" ht="15">
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="15">
       <c r="B51" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" ht="15">
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="15">
       <c r="B53" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" ht="15">
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="15">
       <c r="B55" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" ht="15">
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" ht="15">
       <c r="B57" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" ht="15">
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2108,16 +2312,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="14" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="14" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2128,67 +2334,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>78</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2208,16 +2414,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="15" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="15" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2228,67 +2436,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>79</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2308,16 +2516,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="16" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="16" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2328,67 +2538,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>80</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2408,16 +2618,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="17" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="17" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2428,67 +2640,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>81</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2508,16 +2720,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="18" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="18" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2528,67 +2742,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>82</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2608,16 +2822,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="19" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="19" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2628,71 +2844,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>72</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>68</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>73</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>69</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>74</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>70</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>69</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2712,16 +2936,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="21" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="21" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2732,71 +2958,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>83</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>68</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>84</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>70</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>85</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>71</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>70</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2816,16 +3050,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="22" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="22" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2836,71 +3072,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>88</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>68</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>89</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>87</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>90</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>70</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>87</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2920,16 +3164,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="23" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="23" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2940,71 +3186,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>92</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>68</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>87</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>94</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>69</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>87</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3024,16 +3278,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="24" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="24" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3044,71 +3300,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>96</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>68</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>97</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>69</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>98</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>69</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3128,11 +3392,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" style="5" customWidth="1"/>
@@ -3145,7 +3409,7 @@
     <col min="10" max="16384" width="12.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -3171,31 +3435,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H2" s="32"/>
     </row>
-    <row r="3" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -3205,7 +3469,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -3215,7 +3479,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -3225,7 +3489,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -3235,7 +3499,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -3245,7 +3509,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -3255,7 +3519,7 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -3265,7 +3529,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3288,16 +3552,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="25" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="25" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3308,71 +3574,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>59</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>68</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>60</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>71</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>76</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>70</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>71</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3392,16 +3666,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="26" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="26" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3412,71 +3688,87 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>100</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>68</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>101</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>69</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>102</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>87</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>70</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>87</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>69</v>
+      </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3496,16 +3788,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="27" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="27" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3516,71 +3810,87 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>106</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>68</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>107</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>70</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>108</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>69</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>71</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>69</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>70</v>
+      </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3604,13 +3914,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="6" width="11.44140625" style="28" customWidth="1"/>
     <col min="7" max="16384" width="11.44140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3619,67 +3929,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16.350000000000001" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3700,17 +4010,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="6" width="11.44140625" style="29" customWidth="1"/>
     <col min="7" max="16384" width="11.44140625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3719,67 +4029,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3800,15 +4110,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="6" width="11.44140625" style="30" customWidth="1"/>
     <col min="7" max="16384" width="11.44140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3817,67 +4129,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3898,15 +4210,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="6" width="11.44140625" style="31" customWidth="1"/>
     <col min="7" max="16384" width="11.44140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3915,67 +4229,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3992,22 +4306,117 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
+  <cols>
+    <col min="1" max="6" width="11.44140625" style="31" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="6" width="12.6640625" style="35" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4018,60 +4427,60 @@
       <c r="D1" s="34"/>
       <c r="E1" s="34"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4092,10 +4501,10 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="3" width="16" style="35" customWidth="1"/>
@@ -4103,7 +4512,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4116,68 +4525,68 @@
       <c r="D1" s="33"/>
       <c r="E1" s="34"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4198,10 +4607,10 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="3" width="16" style="35" customWidth="1"/>
@@ -4209,7 +4618,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4224,64 +4633,64 @@
       </c>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>62</v>
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A2" s="50" t="s">
+        <v>122</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4302,10 +4711,10 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="3" width="16" style="35" customWidth="1"/>
@@ -4313,7 +4722,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4328,64 +4737,64 @@
       </c>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4406,10 +4815,10 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="3" width="16" style="35" customWidth="1"/>
@@ -4417,7 +4826,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4432,62 +4841,64 @@
       </c>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>68</v>
+        <v>124</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="34"/>
+        <v>52</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>121</v>
+      </c>
       <c r="D2" s="36" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4508,10 +4919,10 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="17.88671875" style="35" customWidth="1"/>
     <col min="2" max="2" width="16" style="35" customWidth="1"/>
@@ -4521,7 +4932,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4536,64 +4947,64 @@
       </c>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4613,16 +5024,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="13" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="13" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -4633,67 +5046,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>62</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -4702,7 +5115,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51181100000000002" footer="0.51181100000000002"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>